<commit_message>
rebuild derived content and docs
</commit_message>
<xml_diff>
--- a/docs/src/reference/data-dictionaries/C_Dict.xlsx
+++ b/docs/src/reference/data-dictionaries/C_Dict.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD230"/>
+  <dimension ref="A1:AD222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10533,11 +10533,7 @@
       <c r="P135" t="inlineStr"/>
       <c r="Q135" t="inlineStr"/>
       <c r="R135" t="inlineStr"/>
-      <c r="S135" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S135" t="inlineStr"/>
       <c r="T135" t="inlineStr"/>
       <c r="U135" t="inlineStr"/>
       <c r="V135" t="inlineStr">
@@ -10601,11 +10597,7 @@
       <c r="P136" t="inlineStr"/>
       <c r="Q136" t="inlineStr"/>
       <c r="R136" t="inlineStr"/>
-      <c r="S136" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S136" t="inlineStr"/>
       <c r="T136" t="inlineStr"/>
       <c r="U136" t="inlineStr"/>
       <c r="V136" t="inlineStr">
@@ -10669,11 +10661,7 @@
       <c r="P137" t="inlineStr"/>
       <c r="Q137" t="inlineStr"/>
       <c r="R137" t="inlineStr"/>
-      <c r="S137" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S137" t="inlineStr"/>
       <c r="T137" t="inlineStr"/>
       <c r="U137" t="inlineStr"/>
       <c r="V137" t="inlineStr">
@@ -10929,11 +10917,7 @@
       <c r="P141" t="inlineStr"/>
       <c r="Q141" t="inlineStr"/>
       <c r="R141" t="inlineStr"/>
-      <c r="S141" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S141" t="inlineStr"/>
       <c r="T141" t="inlineStr"/>
       <c r="U141" t="inlineStr"/>
       <c r="V141" t="inlineStr">
@@ -10997,11 +10981,7 @@
       <c r="P142" t="inlineStr"/>
       <c r="Q142" t="inlineStr"/>
       <c r="R142" t="inlineStr"/>
-      <c r="S142" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S142" t="inlineStr"/>
       <c r="T142" t="inlineStr"/>
       <c r="U142" t="inlineStr"/>
       <c r="V142" t="inlineStr">
@@ -11065,11 +11045,7 @@
       <c r="P143" t="inlineStr"/>
       <c r="Q143" t="inlineStr"/>
       <c r="R143" t="inlineStr"/>
-      <c r="S143" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S143" t="inlineStr"/>
       <c r="T143" t="inlineStr"/>
       <c r="U143" t="inlineStr"/>
       <c r="V143" t="inlineStr">
@@ -11205,11 +11181,7 @@
       <c r="P145" t="inlineStr"/>
       <c r="Q145" t="inlineStr"/>
       <c r="R145" t="inlineStr"/>
-      <c r="S145" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S145" t="inlineStr"/>
       <c r="T145" t="inlineStr"/>
       <c r="U145" t="inlineStr"/>
       <c r="V145" t="inlineStr">
@@ -11345,11 +11317,7 @@
       <c r="P147" t="inlineStr"/>
       <c r="Q147" t="inlineStr"/>
       <c r="R147" t="inlineStr"/>
-      <c r="S147" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S147" t="inlineStr"/>
       <c r="T147" t="inlineStr"/>
       <c r="U147" t="inlineStr"/>
       <c r="V147" t="inlineStr">
@@ -11485,11 +11453,7 @@
       <c r="P149" t="inlineStr"/>
       <c r="Q149" t="inlineStr"/>
       <c r="R149" t="inlineStr"/>
-      <c r="S149" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S149" t="inlineStr"/>
       <c r="T149" t="inlineStr"/>
       <c r="U149" t="inlineStr"/>
       <c r="V149" t="inlineStr">
@@ -11745,11 +11709,7 @@
       <c r="P153" t="inlineStr"/>
       <c r="Q153" t="inlineStr"/>
       <c r="R153" t="inlineStr"/>
-      <c r="S153" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S153" t="inlineStr"/>
       <c r="T153" t="inlineStr"/>
       <c r="U153" t="inlineStr"/>
       <c r="V153" t="inlineStr">
@@ -11813,11 +11773,7 @@
       <c r="P154" t="inlineStr"/>
       <c r="Q154" t="inlineStr"/>
       <c r="R154" t="inlineStr"/>
-      <c r="S154" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S154" t="inlineStr"/>
       <c r="T154" t="inlineStr"/>
       <c r="U154" t="inlineStr"/>
       <c r="V154" t="inlineStr">
@@ -11881,11 +11837,7 @@
       <c r="P155" t="inlineStr"/>
       <c r="Q155" t="inlineStr"/>
       <c r="R155" t="inlineStr"/>
-      <c r="S155" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S155" t="inlineStr"/>
       <c r="T155" t="inlineStr"/>
       <c r="U155" t="inlineStr"/>
       <c r="V155" t="inlineStr">
@@ -12021,11 +11973,7 @@
       <c r="P157" t="inlineStr"/>
       <c r="Q157" t="inlineStr"/>
       <c r="R157" t="inlineStr"/>
-      <c r="S157" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S157" t="inlineStr"/>
       <c r="T157" t="inlineStr"/>
       <c r="U157" t="inlineStr"/>
       <c r="V157" t="inlineStr">
@@ -12161,11 +12109,7 @@
       <c r="P159" t="inlineStr"/>
       <c r="Q159" t="inlineStr"/>
       <c r="R159" t="inlineStr"/>
-      <c r="S159" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S159" t="inlineStr"/>
       <c r="T159" t="inlineStr"/>
       <c r="U159" t="inlineStr"/>
       <c r="V159" t="inlineStr">
@@ -12301,11 +12245,7 @@
       <c r="P161" t="inlineStr"/>
       <c r="Q161" t="inlineStr"/>
       <c r="R161" t="inlineStr"/>
-      <c r="S161" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S161" t="inlineStr"/>
       <c r="T161" t="inlineStr"/>
       <c r="U161" t="inlineStr"/>
       <c r="V161" t="inlineStr">
@@ -12561,11 +12501,7 @@
       <c r="P165" t="inlineStr"/>
       <c r="Q165" t="inlineStr"/>
       <c r="R165" t="inlineStr"/>
-      <c r="S165" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S165" t="inlineStr"/>
       <c r="T165" t="inlineStr"/>
       <c r="U165" t="inlineStr"/>
       <c r="V165" t="inlineStr">
@@ -12629,11 +12565,7 @@
       <c r="P166" t="inlineStr"/>
       <c r="Q166" t="inlineStr"/>
       <c r="R166" t="inlineStr"/>
-      <c r="S166" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S166" t="inlineStr"/>
       <c r="T166" t="inlineStr"/>
       <c r="U166" t="inlineStr"/>
       <c r="V166" t="inlineStr">
@@ -12697,11 +12629,7 @@
       <c r="P167" t="inlineStr"/>
       <c r="Q167" t="inlineStr"/>
       <c r="R167" t="inlineStr"/>
-      <c r="S167" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S167" t="inlineStr"/>
       <c r="T167" t="inlineStr"/>
       <c r="U167" t="inlineStr"/>
       <c r="V167" t="inlineStr">
@@ -12837,11 +12765,7 @@
       <c r="P169" t="inlineStr"/>
       <c r="Q169" t="inlineStr"/>
       <c r="R169" t="inlineStr"/>
-      <c r="S169" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S169" t="inlineStr"/>
       <c r="T169" t="inlineStr"/>
       <c r="U169" t="inlineStr"/>
       <c r="V169" t="inlineStr">
@@ -12977,11 +12901,7 @@
       <c r="P171" t="inlineStr"/>
       <c r="Q171" t="inlineStr"/>
       <c r="R171" t="inlineStr"/>
-      <c r="S171" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S171" t="inlineStr"/>
       <c r="T171" t="inlineStr"/>
       <c r="U171" t="inlineStr"/>
       <c r="V171" t="inlineStr">
@@ -13117,11 +13037,7 @@
       <c r="P173" t="inlineStr"/>
       <c r="Q173" t="inlineStr"/>
       <c r="R173" t="inlineStr"/>
-      <c r="S173" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S173" t="inlineStr"/>
       <c r="T173" t="inlineStr"/>
       <c r="U173" t="inlineStr"/>
       <c r="V173" t="inlineStr">
@@ -13185,11 +13101,7 @@
       <c r="P174" t="inlineStr"/>
       <c r="Q174" t="inlineStr"/>
       <c r="R174" t="inlineStr"/>
-      <c r="S174" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S174" t="inlineStr"/>
       <c r="T174" t="inlineStr"/>
       <c r="U174" t="inlineStr"/>
       <c r="V174" t="inlineStr">
@@ -13253,11 +13165,7 @@
       <c r="P175" t="inlineStr"/>
       <c r="Q175" t="inlineStr"/>
       <c r="R175" t="inlineStr"/>
-      <c r="S175" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S175" t="inlineStr"/>
       <c r="T175" t="inlineStr"/>
       <c r="U175" t="inlineStr"/>
       <c r="V175" t="inlineStr">
@@ -13321,11 +13229,7 @@
       <c r="P176" t="inlineStr"/>
       <c r="Q176" t="inlineStr"/>
       <c r="R176" t="inlineStr"/>
-      <c r="S176" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S176" t="inlineStr"/>
       <c r="T176" t="inlineStr"/>
       <c r="U176" t="inlineStr"/>
       <c r="V176" t="inlineStr">
@@ -13394,12 +13298,12 @@
       <c r="U177" t="inlineStr"/>
       <c r="V177" t="inlineStr">
         <is>
-          <t>TlBupCtTmBk30</t>
+          <t>TlBupMinDis</t>
         </is>
       </c>
       <c r="W177" t="inlineStr">
         <is>
-          <t>Count of tracts within 30-min telehealth buprenorphine biking range</t>
+          <t>Minimum distance to telehealth buprenorphine provider</t>
         </is>
       </c>
       <c r="X177" t="inlineStr"/>
@@ -13458,12 +13362,12 @@
       <c r="U178" t="inlineStr"/>
       <c r="V178" t="inlineStr">
         <is>
-          <t>TlBupCtTmDr30</t>
+          <t>TlBupTmBk</t>
         </is>
       </c>
       <c r="W178" t="inlineStr">
         <is>
-          <t>Count of tracts within 30-min telehealth buprenorphine driving range</t>
+          <t>Biking time to nearest telehealth buprenorphine provider</t>
         </is>
       </c>
       <c r="X178" t="inlineStr"/>
@@ -13522,12 +13426,12 @@
       <c r="U179" t="inlineStr"/>
       <c r="V179" t="inlineStr">
         <is>
-          <t>TlBupCtTmDr60</t>
+          <t>TlBupTmDr</t>
         </is>
       </c>
       <c r="W179" t="inlineStr">
         <is>
-          <t>Count of tracts within 60-min telehealth buprenorphine driving range</t>
+          <t>Driving time to nearest telehealth buprenorphine provider</t>
         </is>
       </c>
       <c r="X179" t="inlineStr"/>
@@ -13586,12 +13490,12 @@
       <c r="U180" t="inlineStr"/>
       <c r="V180" t="inlineStr">
         <is>
-          <t>TlBupCtTmWk30</t>
+          <t>TlBupTmWk</t>
         </is>
       </c>
       <c r="W180" t="inlineStr">
         <is>
-          <t>Count of tracts within 30-min telehealth buprenorphine walking range</t>
+          <t>Walking time to nearest telehealth buprenorphine provider</t>
         </is>
       </c>
       <c r="X180" t="inlineStr"/>
@@ -13622,7 +13526,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Spatial Access to MOUDs</t>
+          <t>Spatial Access to Mental Health Providers</t>
         </is>
       </c>
       <c r="C181" t="inlineStr"/>
@@ -13636,42 +13540,42 @@
       <c r="K181" t="inlineStr"/>
       <c r="L181" t="inlineStr"/>
       <c r="M181" t="inlineStr"/>
-      <c r="N181" t="inlineStr"/>
+      <c r="N181" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O181" t="inlineStr"/>
       <c r="P181" t="inlineStr"/>
       <c r="Q181" t="inlineStr"/>
       <c r="R181" t="inlineStr"/>
-      <c r="S181" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S181" t="inlineStr"/>
       <c r="T181" t="inlineStr"/>
       <c r="U181" t="inlineStr"/>
       <c r="V181" t="inlineStr">
         <is>
-          <t>TlBupMinDis</t>
+          <t>MhAvTmDr</t>
         </is>
       </c>
       <c r="W181" t="inlineStr">
         <is>
-          <t>Minimum distance to telehealth buprenorphine provider</t>
+          <t>Driving Time (min) to nearest Mental Health Provider</t>
         </is>
       </c>
       <c r="X181" t="inlineStr"/>
       <c r="Y181" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_MOUDs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Mental_Health.md</t>
         </is>
       </c>
       <c r="Z181" t="inlineStr">
         <is>
-          <t>SAMSHA 2019, 2021; Vivitrol 2020; OSRM 2020;</t>
+          <t>SAMHSA 2020</t>
         </is>
       </c>
       <c r="AA181" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2019; Vivitrol, 2020; Open Source Routing Machine, 2020</t>
+          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2020</t>
         </is>
       </c>
       <c r="AB181" t="inlineStr"/>
@@ -13686,7 +13590,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Spatial Access to MOUDs</t>
+          <t>Spatial Access to Mental Health Providers</t>
         </is>
       </c>
       <c r="C182" t="inlineStr"/>
@@ -13700,42 +13604,42 @@
       <c r="K182" t="inlineStr"/>
       <c r="L182" t="inlineStr"/>
       <c r="M182" t="inlineStr"/>
-      <c r="N182" t="inlineStr"/>
+      <c r="N182" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O182" t="inlineStr"/>
       <c r="P182" t="inlineStr"/>
       <c r="Q182" t="inlineStr"/>
       <c r="R182" t="inlineStr"/>
-      <c r="S182" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S182" t="inlineStr"/>
       <c r="T182" t="inlineStr"/>
       <c r="U182" t="inlineStr"/>
       <c r="V182" t="inlineStr">
         <is>
-          <t>TlBupTmBk</t>
+          <t>MhCtTmDr</t>
         </is>
       </c>
       <c r="W182" t="inlineStr">
         <is>
-          <t>Biking time to nearest telehealth buprenorphine provider</t>
+          <t>Tracts with Mental Health Provider (30-min drive)</t>
         </is>
       </c>
       <c r="X182" t="inlineStr"/>
       <c r="Y182" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_MOUDs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Mental_Health.md</t>
         </is>
       </c>
       <c r="Z182" t="inlineStr">
         <is>
-          <t>SAMSHA 2019, 2021; Vivitrol 2020; OSRM 2020;</t>
+          <t>SAMHSA 2020</t>
         </is>
       </c>
       <c r="AA182" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2019; Vivitrol, 2020; Open Source Routing Machine, 2020</t>
+          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2020</t>
         </is>
       </c>
       <c r="AB182" t="inlineStr"/>
@@ -13750,7 +13654,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Spatial Access to MOUDs</t>
+          <t>Spatial Access to Mental Health Providers</t>
         </is>
       </c>
       <c r="C183" t="inlineStr"/>
@@ -13764,42 +13668,42 @@
       <c r="K183" t="inlineStr"/>
       <c r="L183" t="inlineStr"/>
       <c r="M183" t="inlineStr"/>
-      <c r="N183" t="inlineStr"/>
+      <c r="N183" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O183" t="inlineStr"/>
       <c r="P183" t="inlineStr"/>
       <c r="Q183" t="inlineStr"/>
       <c r="R183" t="inlineStr"/>
-      <c r="S183" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S183" t="inlineStr"/>
       <c r="T183" t="inlineStr"/>
       <c r="U183" t="inlineStr"/>
       <c r="V183" t="inlineStr">
         <is>
-          <t>TlBupTmBk30P</t>
+          <t>MhTmDrP</t>
         </is>
       </c>
       <c r="W183" t="inlineStr">
         <is>
-          <t>Percent of tracts within 30-min telehealth buprenorphine biking range</t>
+          <t>% Tracts with Mental Health Provider (30-min drive)</t>
         </is>
       </c>
       <c r="X183" t="inlineStr"/>
       <c r="Y183" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_MOUDs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Mental_Health.md</t>
         </is>
       </c>
       <c r="Z183" t="inlineStr">
         <is>
-          <t>SAMSHA 2019, 2021; Vivitrol 2020; OSRM 2020;</t>
+          <t>SAMHSA 2020</t>
         </is>
       </c>
       <c r="AA183" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2019; Vivitrol, 2020; Open Source Routing Machine, 2020</t>
+          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2020</t>
         </is>
       </c>
       <c r="AB183" t="inlineStr"/>
@@ -13814,7 +13718,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Spatial Access to MOUDs</t>
+          <t>Spatial Access to Pharmacies</t>
         </is>
       </c>
       <c r="C184" t="inlineStr"/>
@@ -13827,43 +13731,43 @@
       <c r="J184" t="inlineStr"/>
       <c r="K184" t="inlineStr"/>
       <c r="L184" t="inlineStr"/>
-      <c r="M184" t="inlineStr"/>
+      <c r="M184" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N184" t="inlineStr"/>
       <c r="O184" t="inlineStr"/>
       <c r="P184" t="inlineStr"/>
       <c r="Q184" t="inlineStr"/>
       <c r="R184" t="inlineStr"/>
-      <c r="S184" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S184" t="inlineStr"/>
       <c r="T184" t="inlineStr"/>
       <c r="U184" t="inlineStr"/>
       <c r="V184" t="inlineStr">
         <is>
-          <t>TlBupTmDr</t>
+          <t>RxAvTmDr</t>
         </is>
       </c>
       <c r="W184" t="inlineStr">
         <is>
-          <t>Driving time to nearest telehealth buprenorphine provider</t>
+          <t xml:space="preserve">Avg. Driving Time (min) to nearest Pharmacy </t>
         </is>
       </c>
       <c r="X184" t="inlineStr"/>
       <c r="Y184" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_MOUDs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Pharmacies.md</t>
         </is>
       </c>
       <c r="Z184" t="inlineStr">
         <is>
-          <t>SAMSHA 2019, 2021; Vivitrol 2020; OSRM 2020;</t>
+          <t>InfoGroup 2019</t>
         </is>
       </c>
       <c r="AA184" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2019; Vivitrol, 2020; Open Source Routing Machine, 2020</t>
+          <t>InfoGroup, 2019</t>
         </is>
       </c>
       <c r="AB184" t="inlineStr"/>
@@ -13878,7 +13782,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Spatial Access to MOUDs</t>
+          <t>Spatial Access to Pharmacies</t>
         </is>
       </c>
       <c r="C185" t="inlineStr"/>
@@ -13891,43 +13795,43 @@
       <c r="J185" t="inlineStr"/>
       <c r="K185" t="inlineStr"/>
       <c r="L185" t="inlineStr"/>
-      <c r="M185" t="inlineStr"/>
+      <c r="M185" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N185" t="inlineStr"/>
       <c r="O185" t="inlineStr"/>
       <c r="P185" t="inlineStr"/>
       <c r="Q185" t="inlineStr"/>
       <c r="R185" t="inlineStr"/>
-      <c r="S185" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S185" t="inlineStr"/>
       <c r="T185" t="inlineStr"/>
       <c r="U185" t="inlineStr"/>
       <c r="V185" t="inlineStr">
         <is>
-          <t>TlBupTmDr30P</t>
+          <t>RxCtTmDr</t>
         </is>
       </c>
       <c r="W185" t="inlineStr">
         <is>
-          <t>Percent of tracts within 30-min telehealth buprenorphine driving range</t>
+          <t>Tracts with Pharmacy (30-min drive)</t>
         </is>
       </c>
       <c r="X185" t="inlineStr"/>
       <c r="Y185" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_MOUDs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Pharmacies.md</t>
         </is>
       </c>
       <c r="Z185" t="inlineStr">
         <is>
-          <t>SAMSHA 2019, 2021; Vivitrol 2020; OSRM 2020;</t>
+          <t>InfoGroup 2019</t>
         </is>
       </c>
       <c r="AA185" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2019; Vivitrol, 2020; Open Source Routing Machine, 2020</t>
+          <t>InfoGroup, 2019</t>
         </is>
       </c>
       <c r="AB185" t="inlineStr"/>
@@ -13942,7 +13846,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Spatial Access to MOUDs</t>
+          <t>Spatial Access to Pharmacies</t>
         </is>
       </c>
       <c r="C186" t="inlineStr"/>
@@ -13955,43 +13859,43 @@
       <c r="J186" t="inlineStr"/>
       <c r="K186" t="inlineStr"/>
       <c r="L186" t="inlineStr"/>
-      <c r="M186" t="inlineStr"/>
+      <c r="M186" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N186" t="inlineStr"/>
       <c r="O186" t="inlineStr"/>
       <c r="P186" t="inlineStr"/>
       <c r="Q186" t="inlineStr"/>
       <c r="R186" t="inlineStr"/>
-      <c r="S186" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S186" t="inlineStr"/>
       <c r="T186" t="inlineStr"/>
       <c r="U186" t="inlineStr"/>
       <c r="V186" t="inlineStr">
         <is>
-          <t>TlBupTmDr60P</t>
+          <t>RxTmDrP</t>
         </is>
       </c>
       <c r="W186" t="inlineStr">
         <is>
-          <t>Percent of tracts within 60-min telehealth buprenorphine driving range</t>
+          <t>% tracts with Pharmacy (30-min drive)</t>
         </is>
       </c>
       <c r="X186" t="inlineStr"/>
       <c r="Y186" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_MOUDs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Pharmacies.md</t>
         </is>
       </c>
       <c r="Z186" t="inlineStr">
         <is>
-          <t>SAMSHA 2019, 2021; Vivitrol 2020; OSRM 2020;</t>
+          <t>InfoGroup 2019</t>
         </is>
       </c>
       <c r="AA186" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2019; Vivitrol, 2020; Open Source Routing Machine, 2020</t>
+          <t>InfoGroup, 2019</t>
         </is>
       </c>
       <c r="AB186" t="inlineStr"/>
@@ -14006,7 +13910,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Spatial Access to MOUDs</t>
+          <t>Spatial Access to Substance Use Treatment Providers</t>
         </is>
       </c>
       <c r="C187" t="inlineStr"/>
@@ -14020,42 +13924,42 @@
       <c r="K187" t="inlineStr"/>
       <c r="L187" t="inlineStr"/>
       <c r="M187" t="inlineStr"/>
-      <c r="N187" t="inlineStr"/>
+      <c r="N187" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O187" t="inlineStr"/>
       <c r="P187" t="inlineStr"/>
       <c r="Q187" t="inlineStr"/>
       <c r="R187" t="inlineStr"/>
-      <c r="S187" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S187" t="inlineStr"/>
       <c r="T187" t="inlineStr"/>
       <c r="U187" t="inlineStr"/>
       <c r="V187" t="inlineStr">
         <is>
-          <t>TlBupTmWk</t>
+          <t>SutpAvTmDr</t>
         </is>
       </c>
       <c r="W187" t="inlineStr">
         <is>
-          <t>Walking time to nearest telehealth buprenorphine provider</t>
+          <t>Driving Time (min) to nearest Substance Use Treatment program</t>
         </is>
       </c>
       <c r="X187" t="inlineStr"/>
       <c r="Y187" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_MOUDs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_SubstanceUseTreatment.md</t>
         </is>
       </c>
       <c r="Z187" t="inlineStr">
         <is>
-          <t>SAMSHA 2019, 2021; Vivitrol 2020; OSRM 2020;</t>
+          <t>SAMHSA 2020</t>
         </is>
       </c>
       <c r="AA187" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2019; Vivitrol, 2020; Open Source Routing Machine, 2020</t>
+          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2020</t>
         </is>
       </c>
       <c r="AB187" t="inlineStr"/>
@@ -14070,7 +13974,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Spatial Access to MOUDs</t>
+          <t>Spatial Access to Substance Use Treatment Providers</t>
         </is>
       </c>
       <c r="C188" t="inlineStr"/>
@@ -14084,42 +13988,42 @@
       <c r="K188" t="inlineStr"/>
       <c r="L188" t="inlineStr"/>
       <c r="M188" t="inlineStr"/>
-      <c r="N188" t="inlineStr"/>
+      <c r="N188" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O188" t="inlineStr"/>
       <c r="P188" t="inlineStr"/>
       <c r="Q188" t="inlineStr"/>
       <c r="R188" t="inlineStr"/>
-      <c r="S188" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S188" t="inlineStr"/>
       <c r="T188" t="inlineStr"/>
       <c r="U188" t="inlineStr"/>
       <c r="V188" t="inlineStr">
         <is>
-          <t>TlBupTmWk30P</t>
+          <t>SutpCtTmDr</t>
         </is>
       </c>
       <c r="W188" t="inlineStr">
         <is>
-          <t>Percent of tracts within 30-min telehealth buprenorphine walking range</t>
+          <t>Tracts with Substance Use Treatment (SUT) program (30-min drive)</t>
         </is>
       </c>
       <c r="X188" t="inlineStr"/>
       <c r="Y188" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_MOUDs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_SubstanceUseTreatment.md</t>
         </is>
       </c>
       <c r="Z188" t="inlineStr">
         <is>
-          <t>SAMSHA 2019, 2021; Vivitrol 2020; OSRM 2020;</t>
+          <t>SAMHSA 2020</t>
         </is>
       </c>
       <c r="AA188" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2019; Vivitrol, 2020; Open Source Routing Machine, 2020</t>
+          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2020</t>
         </is>
       </c>
       <c r="AB188" t="inlineStr"/>
@@ -14134,7 +14038,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Spatial Access to Mental Health Providers</t>
+          <t>Spatial Access to Substance Use Treatment Providers</t>
         </is>
       </c>
       <c r="C189" t="inlineStr"/>
@@ -14157,27 +14061,23 @@
       <c r="P189" t="inlineStr"/>
       <c r="Q189" t="inlineStr"/>
       <c r="R189" t="inlineStr"/>
-      <c r="S189" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S189" t="inlineStr"/>
       <c r="T189" t="inlineStr"/>
       <c r="U189" t="inlineStr"/>
       <c r="V189" t="inlineStr">
         <is>
-          <t>MhAvTmDr</t>
+          <t>SutpTmDrP</t>
         </is>
       </c>
       <c r="W189" t="inlineStr">
         <is>
-          <t>Driving Time (min) to nearest Mental Health Provider</t>
+          <t>% tracts with Substance Use Treatment program (30-min drive)</t>
         </is>
       </c>
       <c r="X189" t="inlineStr"/>
       <c r="Y189" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Mental_Health.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_SubstanceUseTreatment.md</t>
         </is>
       </c>
       <c r="Z189" t="inlineStr">
@@ -14202,7 +14102,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Spatial Access to Mental Health Providers</t>
+          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
         </is>
       </c>
       <c r="C190" t="inlineStr"/>
@@ -14234,28 +14134,28 @@
       <c r="U190" t="inlineStr"/>
       <c r="V190" t="inlineStr">
         <is>
-          <t>MhCtTmDr</t>
+          <t>FqhcAvTmDr</t>
         </is>
       </c>
       <c r="W190" t="inlineStr">
         <is>
-          <t>Tracts with Mental Health Provider (30-min drive)</t>
+          <t>Average driving time to nearest Federally Qualified Health Center (FQHC)</t>
         </is>
       </c>
       <c r="X190" t="inlineStr"/>
       <c r="Y190" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Mental_Health.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
         </is>
       </c>
       <c r="Z190" t="inlineStr">
         <is>
-          <t>SAMHSA 2020</t>
+          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
         </is>
       </c>
       <c r="AA190" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2020</t>
+          <t>United States Covid Atlas via Health Resources and Services Administration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
         </is>
       </c>
       <c r="AB190" t="inlineStr"/>
@@ -14270,7 +14170,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Spatial Access to Mental Health Providers</t>
+          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
         </is>
       </c>
       <c r="C191" t="inlineStr"/>
@@ -14284,11 +14184,7 @@
       <c r="K191" t="inlineStr"/>
       <c r="L191" t="inlineStr"/>
       <c r="M191" t="inlineStr"/>
-      <c r="N191" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N191" t="inlineStr"/>
       <c r="O191" t="inlineStr"/>
       <c r="P191" t="inlineStr"/>
       <c r="Q191" t="inlineStr"/>
@@ -14298,32 +14194,36 @@
           <t>x</t>
         </is>
       </c>
-      <c r="T191" t="inlineStr"/>
+      <c r="T191" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U191" t="inlineStr"/>
       <c r="V191" t="inlineStr">
         <is>
-          <t>MhTmDrP</t>
+          <t>FqhcAvTmDr2</t>
         </is>
       </c>
       <c r="W191" t="inlineStr">
         <is>
-          <t>% Tracts with Mental Health Provider (30-min drive)</t>
+          <t>Average driving time to nearest Federally Qualified Health Center (FQHC), with Impedance factor</t>
         </is>
       </c>
       <c r="X191" t="inlineStr"/>
       <c r="Y191" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Mental_Health.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
         </is>
       </c>
       <c r="Z191" t="inlineStr">
         <is>
-          <t>SAMHSA 2020</t>
+          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
         </is>
       </c>
       <c r="AA191" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2020</t>
+          <t>United States Covid Atlas via Health Resources and Services Administration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
         </is>
       </c>
       <c r="AB191" t="inlineStr"/>
@@ -14338,7 +14238,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Spatial Access to Pharmacies</t>
+          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
         </is>
       </c>
       <c r="C192" t="inlineStr"/>
@@ -14351,43 +14251,47 @@
       <c r="J192" t="inlineStr"/>
       <c r="K192" t="inlineStr"/>
       <c r="L192" t="inlineStr"/>
-      <c r="M192" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N192" t="inlineStr"/>
+      <c r="M192" t="inlineStr"/>
+      <c r="N192" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O192" t="inlineStr"/>
       <c r="P192" t="inlineStr"/>
       <c r="Q192" t="inlineStr"/>
       <c r="R192" t="inlineStr"/>
-      <c r="S192" t="inlineStr"/>
+      <c r="S192" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T192" t="inlineStr"/>
       <c r="U192" t="inlineStr"/>
       <c r="V192" t="inlineStr">
         <is>
-          <t>RxAvTmDr</t>
+          <t>FqhcCtTmDr</t>
         </is>
       </c>
       <c r="W192" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avg. Driving Time (min) to nearest Pharmacy </t>
+          <t>Count of Tracts within 30-min drive of Federally Qualified Health Center (FQHC)</t>
         </is>
       </c>
       <c r="X192" t="inlineStr"/>
       <c r="Y192" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Pharmacies.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
         </is>
       </c>
       <c r="Z192" t="inlineStr">
         <is>
-          <t>InfoGroup 2019</t>
+          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
         </is>
       </c>
       <c r="AA192" t="inlineStr">
         <is>
-          <t>InfoGroup, 2019</t>
+          <t>United States Covid Atlas via Health Resources and Services Administration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
         </is>
       </c>
       <c r="AB192" t="inlineStr"/>
@@ -14402,7 +14306,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Spatial Access to Pharmacies</t>
+          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
         </is>
       </c>
       <c r="C193" t="inlineStr"/>
@@ -14415,43 +14319,43 @@
       <c r="J193" t="inlineStr"/>
       <c r="K193" t="inlineStr"/>
       <c r="L193" t="inlineStr"/>
-      <c r="M193" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M193" t="inlineStr"/>
       <c r="N193" t="inlineStr"/>
       <c r="O193" t="inlineStr"/>
       <c r="P193" t="inlineStr"/>
       <c r="Q193" t="inlineStr"/>
       <c r="R193" t="inlineStr"/>
-      <c r="S193" t="inlineStr"/>
+      <c r="S193" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T193" t="inlineStr"/>
       <c r="U193" t="inlineStr"/>
       <c r="V193" t="inlineStr">
         <is>
-          <t>RxCtTmDr</t>
+          <t>FqhcCtTmDr2</t>
         </is>
       </c>
       <c r="W193" t="inlineStr">
         <is>
-          <t>Tracts with Pharmacy (30-min drive)</t>
+          <t>Count of Tracts within 30-min drive of Federally Qualified Health Center (FQHC), with Impedance factor</t>
         </is>
       </c>
       <c r="X193" t="inlineStr"/>
       <c r="Y193" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Pharmacies.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
         </is>
       </c>
       <c r="Z193" t="inlineStr">
         <is>
-          <t>InfoGroup 2019</t>
+          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
         </is>
       </c>
       <c r="AA193" t="inlineStr">
         <is>
-          <t>InfoGroup, 2019</t>
+          <t>United States Covid Atlas via Health Resources and Services Administration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
         </is>
       </c>
       <c r="AB193" t="inlineStr"/>
@@ -14466,7 +14370,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Spatial Access to Pharmacies</t>
+          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
         </is>
       </c>
       <c r="C194" t="inlineStr"/>
@@ -14479,43 +14383,47 @@
       <c r="J194" t="inlineStr"/>
       <c r="K194" t="inlineStr"/>
       <c r="L194" t="inlineStr"/>
-      <c r="M194" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N194" t="inlineStr"/>
+      <c r="M194" t="inlineStr"/>
+      <c r="N194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O194" t="inlineStr"/>
       <c r="P194" t="inlineStr"/>
       <c r="Q194" t="inlineStr"/>
       <c r="R194" t="inlineStr"/>
-      <c r="S194" t="inlineStr"/>
+      <c r="S194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T194" t="inlineStr"/>
       <c r="U194" t="inlineStr"/>
       <c r="V194" t="inlineStr">
         <is>
-          <t>RxTmDrP</t>
+          <t>FqhcTmDrP</t>
         </is>
       </c>
       <c r="W194" t="inlineStr">
         <is>
-          <t>% tracts with Pharmacy (30-min drive)</t>
+          <t>% Tracts within 30-min drive of Federally Qualified Health Center (FQHC)</t>
         </is>
       </c>
       <c r="X194" t="inlineStr"/>
       <c r="Y194" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_Pharmacies.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
         </is>
       </c>
       <c r="Z194" t="inlineStr">
         <is>
-          <t>InfoGroup 2019</t>
+          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
         </is>
       </c>
       <c r="AA194" t="inlineStr">
         <is>
-          <t>InfoGroup, 2019</t>
+          <t>United States Covid Atlas via Health Resources and Services Administration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
         </is>
       </c>
       <c r="AB194" t="inlineStr"/>
@@ -14530,7 +14438,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Spatial Access to Substance Use Treatment Providers</t>
+          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
         </is>
       </c>
       <c r="C195" t="inlineStr"/>
@@ -14544,42 +14452,46 @@
       <c r="K195" t="inlineStr"/>
       <c r="L195" t="inlineStr"/>
       <c r="M195" t="inlineStr"/>
-      <c r="N195" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N195" t="inlineStr"/>
       <c r="O195" t="inlineStr"/>
       <c r="P195" t="inlineStr"/>
       <c r="Q195" t="inlineStr"/>
       <c r="R195" t="inlineStr"/>
-      <c r="S195" t="inlineStr"/>
-      <c r="T195" t="inlineStr"/>
+      <c r="S195" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="T195" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U195" t="inlineStr"/>
       <c r="V195" t="inlineStr">
         <is>
-          <t>SutpAvTmDr</t>
+          <t>FqhcTmDrP2</t>
         </is>
       </c>
       <c r="W195" t="inlineStr">
         <is>
-          <t>Driving Time (min) to nearest Substance Use Treatment program</t>
+          <t>% Tracts within 30-min drive of Federally Qualified Health Center (FQHC), with Impedance factor</t>
         </is>
       </c>
       <c r="X195" t="inlineStr"/>
       <c r="Y195" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_SubstanceUseTreatment.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
         </is>
       </c>
       <c r="Z195" t="inlineStr">
         <is>
-          <t>SAMHSA 2020</t>
+          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
         </is>
       </c>
       <c r="AA195" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2020</t>
+          <t>United States Covid Atlas via Health Resources and Services Administration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
         </is>
       </c>
       <c r="AB195" t="inlineStr"/>
@@ -14594,7 +14506,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Spatial Access to Substance Use Treatment Providers</t>
+          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
         </is>
       </c>
       <c r="C196" t="inlineStr"/>
@@ -14606,44 +14518,48 @@
       <c r="I196" t="inlineStr"/>
       <c r="J196" t="inlineStr"/>
       <c r="K196" t="inlineStr"/>
-      <c r="L196" t="inlineStr"/>
+      <c r="L196" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M196" t="inlineStr"/>
-      <c r="N196" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N196" t="inlineStr"/>
       <c r="O196" t="inlineStr"/>
       <c r="P196" t="inlineStr"/>
       <c r="Q196" t="inlineStr"/>
       <c r="R196" t="inlineStr"/>
-      <c r="S196" t="inlineStr"/>
+      <c r="S196" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T196" t="inlineStr"/>
       <c r="U196" t="inlineStr"/>
       <c r="V196" t="inlineStr">
         <is>
-          <t>SutpCtTmDr</t>
+          <t>TotTracts</t>
         </is>
       </c>
       <c r="W196" t="inlineStr">
         <is>
-          <t>Tracts with Substance Use Treatment (SUT) program (30-min drive)</t>
+          <t>Total Census Tract Count</t>
         </is>
       </c>
       <c r="X196" t="inlineStr"/>
       <c r="Y196" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_SubstanceUseTreatment.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
         </is>
       </c>
       <c r="Z196" t="inlineStr">
         <is>
-          <t>SAMHSA 2020</t>
+          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
         </is>
       </c>
       <c r="AA196" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2020</t>
+          <t>United States Covid Atlas via Health Resources and Services Administration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
         </is>
       </c>
       <c r="AB196" t="inlineStr"/>
@@ -14658,7 +14574,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Spatial Access to Substance Use Treatment Providers</t>
+          <t>Urban/Suburban/Rural Classification</t>
         </is>
       </c>
       <c r="C197" t="inlineStr"/>
@@ -14670,13 +14586,13 @@
       <c r="I197" t="inlineStr"/>
       <c r="J197" t="inlineStr"/>
       <c r="K197" t="inlineStr"/>
-      <c r="L197" t="inlineStr"/>
+      <c r="L197" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M197" t="inlineStr"/>
-      <c r="N197" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N197" t="inlineStr"/>
       <c r="O197" t="inlineStr"/>
       <c r="P197" t="inlineStr"/>
       <c r="Q197" t="inlineStr"/>
@@ -14686,28 +14602,28 @@
       <c r="U197" t="inlineStr"/>
       <c r="V197" t="inlineStr">
         <is>
-          <t>SutpTmDrP</t>
+          <t>CenFlags</t>
         </is>
       </c>
       <c r="W197" t="inlineStr">
         <is>
-          <t>% tracts with Substance Use Treatment program (30-min drive)</t>
+          <t>Census Flags</t>
         </is>
       </c>
       <c r="X197" t="inlineStr"/>
       <c r="Y197" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_SubstanceUseTreatment.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Urbanicity.md</t>
         </is>
       </c>
       <c r="Z197" t="inlineStr">
         <is>
-          <t>SAMHSA 2020</t>
+          <t>USDA-ERS 2010; ACS 2018</t>
         </is>
       </c>
       <c r="AA197" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2020</t>
+          <t>United States Department of Agriculture Economic Research Service, 2010; American Community Survey 2014-2018 5-Year Estimate</t>
         </is>
       </c>
       <c r="AB197" t="inlineStr"/>
@@ -14722,7 +14638,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
+          <t>Urban/Suburban/Rural Classification</t>
         </is>
       </c>
       <c r="C198" t="inlineStr"/>
@@ -14734,48 +14650,44 @@
       <c r="I198" t="inlineStr"/>
       <c r="J198" t="inlineStr"/>
       <c r="K198" t="inlineStr"/>
-      <c r="L198" t="inlineStr"/>
+      <c r="L198" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M198" t="inlineStr"/>
-      <c r="N198" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N198" t="inlineStr"/>
       <c r="O198" t="inlineStr"/>
       <c r="P198" t="inlineStr"/>
       <c r="Q198" t="inlineStr"/>
       <c r="R198" t="inlineStr"/>
-      <c r="S198" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S198" t="inlineStr"/>
       <c r="T198" t="inlineStr"/>
       <c r="U198" t="inlineStr"/>
       <c r="V198" t="inlineStr">
         <is>
-          <t>FqhcAvTmDr</t>
+          <t>RcaRuralP</t>
         </is>
       </c>
       <c r="W198" t="inlineStr">
         <is>
-          <t>Average driving time to nearest Federally Qualified Health Center (FQHC)</t>
+          <t>% Tracts Rural (RUCA)</t>
         </is>
       </c>
       <c r="X198" t="inlineStr"/>
       <c r="Y198" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Urbanicity.md</t>
         </is>
       </c>
       <c r="Z198" t="inlineStr">
         <is>
-          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
+          <t>USDA-ERS 2010; ACS 2018</t>
         </is>
       </c>
       <c r="AA198" t="inlineStr">
         <is>
-          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
+          <t>United States Department of Agriculture Economic Research Service, 2010; American Community Survey 2014-2018 5-Year Estimate</t>
         </is>
       </c>
       <c r="AB198" t="inlineStr"/>
@@ -14790,7 +14702,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
+          <t>Urban/Suburban/Rural Classification</t>
         </is>
       </c>
       <c r="C199" t="inlineStr"/>
@@ -14802,48 +14714,44 @@
       <c r="I199" t="inlineStr"/>
       <c r="J199" t="inlineStr"/>
       <c r="K199" t="inlineStr"/>
-      <c r="L199" t="inlineStr"/>
+      <c r="L199" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M199" t="inlineStr"/>
       <c r="N199" t="inlineStr"/>
       <c r="O199" t="inlineStr"/>
       <c r="P199" t="inlineStr"/>
       <c r="Q199" t="inlineStr"/>
       <c r="R199" t="inlineStr"/>
-      <c r="S199" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="T199" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S199" t="inlineStr"/>
+      <c r="T199" t="inlineStr"/>
       <c r="U199" t="inlineStr"/>
       <c r="V199" t="inlineStr">
         <is>
-          <t>FqhcAvTmDr2</t>
+          <t>RcaSubrbP</t>
         </is>
       </c>
       <c r="W199" t="inlineStr">
         <is>
-          <t>Average driving time to nearest Federally Qualified Health Center (FQHC), with Impedance factor</t>
+          <t>% Tracts Suburban (RUCA)</t>
         </is>
       </c>
       <c r="X199" t="inlineStr"/>
       <c r="Y199" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Urbanicity.md</t>
         </is>
       </c>
       <c r="Z199" t="inlineStr">
         <is>
-          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
+          <t>USDA-ERS 2010; ACS 2018</t>
         </is>
       </c>
       <c r="AA199" t="inlineStr">
         <is>
-          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
+          <t>United States Department of Agriculture Economic Research Service, 2010; American Community Survey 2014-2018 5-Year Estimate</t>
         </is>
       </c>
       <c r="AB199" t="inlineStr"/>
@@ -14858,7 +14766,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
+          <t>Urban/Suburban/Rural Classification</t>
         </is>
       </c>
       <c r="C200" t="inlineStr"/>
@@ -14870,48 +14778,44 @@
       <c r="I200" t="inlineStr"/>
       <c r="J200" t="inlineStr"/>
       <c r="K200" t="inlineStr"/>
-      <c r="L200" t="inlineStr"/>
+      <c r="L200" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M200" t="inlineStr"/>
-      <c r="N200" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N200" t="inlineStr"/>
       <c r="O200" t="inlineStr"/>
       <c r="P200" t="inlineStr"/>
       <c r="Q200" t="inlineStr"/>
       <c r="R200" t="inlineStr"/>
-      <c r="S200" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S200" t="inlineStr"/>
       <c r="T200" t="inlineStr"/>
       <c r="U200" t="inlineStr"/>
       <c r="V200" t="inlineStr">
         <is>
-          <t>FqhcCtTmDr</t>
+          <t>RcaUrbanP</t>
         </is>
       </c>
       <c r="W200" t="inlineStr">
         <is>
-          <t>Count of Tracts within 30-min drive of Federally Qualified Health Center (FQHC)</t>
+          <t>% Tracts Urban (RUCA)</t>
         </is>
       </c>
       <c r="X200" t="inlineStr"/>
       <c r="Y200" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Urbanicity.md</t>
         </is>
       </c>
       <c r="Z200" t="inlineStr">
         <is>
-          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
+          <t>USDA-ERS 2010; ACS 2018</t>
         </is>
       </c>
       <c r="AA200" t="inlineStr">
         <is>
-          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
+          <t>United States Department of Agriculture Economic Research Service, 2010; American Community Survey 2014-2018 5-Year Estimate</t>
         </is>
       </c>
       <c r="AB200" t="inlineStr"/>
@@ -14921,12 +14825,12 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Environment</t>
+          <t>Economic</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
+          <t>Employment Trends</t>
         </is>
       </c>
       <c r="C201" t="inlineStr"/>
@@ -14938,44 +14842,44 @@
       <c r="I201" t="inlineStr"/>
       <c r="J201" t="inlineStr"/>
       <c r="K201" t="inlineStr"/>
-      <c r="L201" t="inlineStr"/>
+      <c r="L201" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M201" t="inlineStr"/>
       <c r="N201" t="inlineStr"/>
       <c r="O201" t="inlineStr"/>
       <c r="P201" t="inlineStr"/>
       <c r="Q201" t="inlineStr"/>
       <c r="R201" t="inlineStr"/>
-      <c r="S201" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S201" t="inlineStr"/>
       <c r="T201" t="inlineStr"/>
       <c r="U201" t="inlineStr"/>
       <c r="V201" t="inlineStr">
         <is>
-          <t>FqhcCtTmDr2</t>
+          <t>EssnWrkE</t>
         </is>
       </c>
       <c r="W201" t="inlineStr">
         <is>
-          <t>Count of Tracts within 30-min drive of Federally Qualified Health Center (FQHC), with Impedance factor</t>
+          <t>Count of Essential Workers</t>
         </is>
       </c>
       <c r="X201" t="inlineStr"/>
       <c r="Y201" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
         </is>
       </c>
       <c r="Z201" t="inlineStr">
         <is>
-          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
+          <t>ACS 2018, 2023</t>
         </is>
       </c>
       <c r="AA201" t="inlineStr">
         <is>
-          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
+          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
         </is>
       </c>
       <c r="AB201" t="inlineStr"/>
@@ -14985,12 +14889,12 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Environment</t>
+          <t>Economic</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
+          <t>Employment Trends</t>
         </is>
       </c>
       <c r="C202" t="inlineStr"/>
@@ -15002,7 +14906,11 @@
       <c r="I202" t="inlineStr"/>
       <c r="J202" t="inlineStr"/>
       <c r="K202" t="inlineStr"/>
-      <c r="L202" t="inlineStr"/>
+      <c r="L202" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M202" t="inlineStr"/>
       <c r="N202" t="inlineStr">
         <is>
@@ -15011,39 +14919,39 @@
       </c>
       <c r="O202" t="inlineStr"/>
       <c r="P202" t="inlineStr"/>
-      <c r="Q202" t="inlineStr"/>
+      <c r="Q202" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R202" t="inlineStr"/>
-      <c r="S202" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S202" t="inlineStr"/>
       <c r="T202" t="inlineStr"/>
       <c r="U202" t="inlineStr"/>
       <c r="V202" t="inlineStr">
         <is>
-          <t>FqhcTmDrP</t>
+          <t>EssnWrkP</t>
         </is>
       </c>
       <c r="W202" t="inlineStr">
         <is>
-          <t>% Tracts within 30-min drive of Federally Qualified Health Center (FQHC)</t>
+          <t>Essential Workers %</t>
         </is>
       </c>
       <c r="X202" t="inlineStr"/>
       <c r="Y202" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
         </is>
       </c>
       <c r="Z202" t="inlineStr">
         <is>
-          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
+          <t>ACS 2018, 2023</t>
         </is>
       </c>
       <c r="AA202" t="inlineStr">
         <is>
-          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
+          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
         </is>
       </c>
       <c r="AB202" t="inlineStr"/>
@@ -15053,12 +14961,12 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Environment</t>
+          <t>Economic</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
+          <t>Employment Trends</t>
         </is>
       </c>
       <c r="C203" t="inlineStr"/>
@@ -15070,48 +14978,52 @@
       <c r="I203" t="inlineStr"/>
       <c r="J203" t="inlineStr"/>
       <c r="K203" t="inlineStr"/>
-      <c r="L203" t="inlineStr"/>
+      <c r="L203" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M203" t="inlineStr"/>
-      <c r="N203" t="inlineStr"/>
+      <c r="N203" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O203" t="inlineStr"/>
       <c r="P203" t="inlineStr"/>
-      <c r="Q203" t="inlineStr"/>
+      <c r="Q203" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R203" t="inlineStr"/>
-      <c r="S203" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="T203" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S203" t="inlineStr"/>
+      <c r="T203" t="inlineStr"/>
       <c r="U203" t="inlineStr"/>
       <c r="V203" t="inlineStr">
         <is>
-          <t>FqhcTmDrP2</t>
+          <t>HghRskP</t>
         </is>
       </c>
       <c r="W203" t="inlineStr">
         <is>
-          <t>% Tracts within 30-min drive of Federally Qualified Health Center (FQHC), with Impedance factor</t>
+          <t>Employed % - High Risk of Injury</t>
         </is>
       </c>
       <c r="X203" t="inlineStr"/>
       <c r="Y203" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
         </is>
       </c>
       <c r="Z203" t="inlineStr">
         <is>
-          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
+          <t>ACS 2018, 2023</t>
         </is>
       </c>
       <c r="AA203" t="inlineStr">
         <is>
-          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
+          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
         </is>
       </c>
       <c r="AB203" t="inlineStr"/>
@@ -15121,12 +15033,12 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Environment</t>
+          <t>Economic</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
+          <t>Employment Trends</t>
         </is>
       </c>
       <c r="C204" t="inlineStr"/>
@@ -15144,42 +15056,46 @@
         </is>
       </c>
       <c r="M204" t="inlineStr"/>
-      <c r="N204" t="inlineStr"/>
+      <c r="N204" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O204" t="inlineStr"/>
       <c r="P204" t="inlineStr"/>
-      <c r="Q204" t="inlineStr"/>
+      <c r="Q204" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R204" t="inlineStr"/>
-      <c r="S204" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S204" t="inlineStr"/>
       <c r="T204" t="inlineStr"/>
       <c r="U204" t="inlineStr"/>
       <c r="V204" t="inlineStr">
         <is>
-          <t>TotTracts</t>
+          <t>HltCrP</t>
         </is>
       </c>
       <c r="W204" t="inlineStr">
         <is>
-          <t>Total Census Tract Count</t>
+          <t>Employed % - Health Care</t>
         </is>
       </c>
       <c r="X204" t="inlineStr"/>
       <c r="Y204" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
         </is>
       </c>
       <c r="Z204" t="inlineStr">
         <is>
-          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
+          <t>ACS 2018, 2023</t>
         </is>
       </c>
       <c r="AA204" t="inlineStr">
         <is>
-          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
+          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
         </is>
       </c>
       <c r="AB204" t="inlineStr"/>
@@ -15189,12 +15105,12 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Environment</t>
+          <t>Economic</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Urban/Suburban/Rural Classification</t>
+          <t>Employment Trends</t>
         </is>
       </c>
       <c r="C205" t="inlineStr"/>
@@ -15212,38 +15128,46 @@
         </is>
       </c>
       <c r="M205" t="inlineStr"/>
-      <c r="N205" t="inlineStr"/>
+      <c r="N205" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O205" t="inlineStr"/>
       <c r="P205" t="inlineStr"/>
-      <c r="Q205" t="inlineStr"/>
+      <c r="Q205" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R205" t="inlineStr"/>
       <c r="S205" t="inlineStr"/>
       <c r="T205" t="inlineStr"/>
       <c r="U205" t="inlineStr"/>
       <c r="V205" t="inlineStr">
         <is>
-          <t>CenFlags</t>
+          <t>RetailP</t>
         </is>
       </c>
       <c r="W205" t="inlineStr">
         <is>
-          <t>Census Flags</t>
+          <t>Employed % - Retail</t>
         </is>
       </c>
       <c r="X205" t="inlineStr"/>
       <c r="Y205" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Urbanicity.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
         </is>
       </c>
       <c r="Z205" t="inlineStr">
         <is>
-          <t>USDA-ERS 2010; ACS 2018</t>
+          <t>ACS 2018, 2023</t>
         </is>
       </c>
       <c r="AA205" t="inlineStr">
         <is>
-          <t>United States Department of Agriculture Economic Research Service, 2010; American Community Survey 2014-2018 5-Year Estimate</t>
+          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
         </is>
       </c>
       <c r="AB205" t="inlineStr"/>
@@ -15253,12 +15177,12 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Environment</t>
+          <t>Economic</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Urban/Suburban/Rural Classification</t>
+          <t>Employment Trends</t>
         </is>
       </c>
       <c r="C206" t="inlineStr"/>
@@ -15276,38 +15200,46 @@
         </is>
       </c>
       <c r="M206" t="inlineStr"/>
-      <c r="N206" t="inlineStr"/>
+      <c r="N206" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O206" t="inlineStr"/>
       <c r="P206" t="inlineStr"/>
-      <c r="Q206" t="inlineStr"/>
+      <c r="Q206" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R206" t="inlineStr"/>
       <c r="S206" t="inlineStr"/>
       <c r="T206" t="inlineStr"/>
       <c r="U206" t="inlineStr"/>
       <c r="V206" t="inlineStr">
         <is>
-          <t>RcaRuralP</t>
+          <t>TotWrkE</t>
         </is>
       </c>
       <c r="W206" t="inlineStr">
         <is>
-          <t>% Tracts Rural (RUCA)</t>
+          <t>Count of Working Population</t>
         </is>
       </c>
       <c r="X206" t="inlineStr"/>
       <c r="Y206" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Urbanicity.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
         </is>
       </c>
       <c r="Z206" t="inlineStr">
         <is>
-          <t>USDA-ERS 2010; ACS 2018</t>
+          <t>ACS 2018, 2023</t>
         </is>
       </c>
       <c r="AA206" t="inlineStr">
         <is>
-          <t>United States Department of Agriculture Economic Research Service, 2010; American Community Survey 2014-2018 5-Year Estimate</t>
+          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
         </is>
       </c>
       <c r="AB206" t="inlineStr"/>
@@ -15317,12 +15249,12 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Environment</t>
+          <t>Economic</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Urban/Suburban/Rural Classification</t>
+          <t>Great Recession Foreclosure Rate</t>
         </is>
       </c>
       <c r="C207" t="inlineStr"/>
@@ -15350,28 +15282,28 @@
       <c r="U207" t="inlineStr"/>
       <c r="V207" t="inlineStr">
         <is>
-          <t>RcaSubrbP</t>
+          <t>ForDqP</t>
         </is>
       </c>
       <c r="W207" t="inlineStr">
         <is>
-          <t>% Tracts Suburban (RUCA)</t>
+          <t>Foreclosure &amp; Delinquency %</t>
         </is>
       </c>
       <c r="X207" t="inlineStr"/>
       <c r="Y207" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Urbanicity.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Foreclosure_Rate.md</t>
         </is>
       </c>
       <c r="Z207" t="inlineStr">
         <is>
-          <t>USDA-ERS 2010; ACS 2018</t>
+          <t>HUD 2018; ACS 2012, 2018</t>
         </is>
       </c>
       <c r="AA207" t="inlineStr">
         <is>
-          <t>United States Department of Agriculture Economic Research Service, 2010; American Community Survey 2014-2018 5-Year Estimate</t>
+          <t>U.S. Department of Housing and Urban Development Neighborhood Stabilization Program; American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates</t>
         </is>
       </c>
       <c r="AB207" t="inlineStr"/>
@@ -15381,12 +15313,12 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Environment</t>
+          <t>Economic</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Urban/Suburban/Rural Classification</t>
+          <t>Great Recession Foreclosure Rate</t>
         </is>
       </c>
       <c r="C208" t="inlineStr"/>
@@ -15414,28 +15346,28 @@
       <c r="U208" t="inlineStr"/>
       <c r="V208" t="inlineStr">
         <is>
-          <t>RcaUrbanP</t>
+          <t>ForDqTot</t>
         </is>
       </c>
       <c r="W208" t="inlineStr">
         <is>
-          <t>% Tracts Urban (RUCA)</t>
+          <t>Foreclosure &amp; Delinquency Count</t>
         </is>
       </c>
       <c r="X208" t="inlineStr"/>
       <c r="Y208" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Urbanicity.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Foreclosure_Rate.md</t>
         </is>
       </c>
       <c r="Z208" t="inlineStr">
         <is>
-          <t>USDA-ERS 2010; ACS 2018</t>
+          <t>HUD 2018; ACS 2012, 2018</t>
         </is>
       </c>
       <c r="AA208" t="inlineStr">
         <is>
-          <t>United States Department of Agriculture Economic Research Service, 2010; American Community Survey 2014-2018 5-Year Estimate</t>
+          <t>U.S. Department of Housing and Urban Development Neighborhood Stabilization Program; American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates</t>
         </is>
       </c>
       <c r="AB208" t="inlineStr"/>
@@ -15450,13 +15382,17 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Employment Trends</t>
+          <t>Great Recession Foreclosure Rate</t>
         </is>
       </c>
       <c r="C209" t="inlineStr"/>
       <c r="D209" t="inlineStr"/>
       <c r="E209" t="inlineStr"/>
-      <c r="F209" t="inlineStr"/>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G209" t="inlineStr"/>
       <c r="H209" t="inlineStr"/>
       <c r="I209" t="inlineStr"/>
@@ -15468,38 +15404,46 @@
         </is>
       </c>
       <c r="M209" t="inlineStr"/>
-      <c r="N209" t="inlineStr"/>
+      <c r="N209" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O209" t="inlineStr"/>
       <c r="P209" t="inlineStr"/>
-      <c r="Q209" t="inlineStr"/>
+      <c r="Q209" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R209" t="inlineStr"/>
       <c r="S209" t="inlineStr"/>
       <c r="T209" t="inlineStr"/>
       <c r="U209" t="inlineStr"/>
       <c r="V209" t="inlineStr">
         <is>
-          <t>EssnWrkE</t>
+          <t>GiniCoeff</t>
         </is>
       </c>
       <c r="W209" t="inlineStr">
         <is>
-          <t>Count of Essential Workers</t>
+          <t>Income Inequality (Gini Coefficient)</t>
         </is>
       </c>
       <c r="X209" t="inlineStr"/>
       <c r="Y209" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Foreclosure_Rate.md</t>
         </is>
       </c>
       <c r="Z209" t="inlineStr">
         <is>
-          <t>ACS 2018, 2023</t>
+          <t>HUD 2018; ACS 2012, 2018</t>
         </is>
       </c>
       <c r="AA209" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
+          <t>U.S. Department of Housing and Urban Development Neighborhood Stabilization Program; American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates</t>
         </is>
       </c>
       <c r="AB209" t="inlineStr"/>
@@ -15514,7 +15458,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Employment Trends</t>
+          <t>Internet Access</t>
         </is>
       </c>
       <c r="C210" t="inlineStr"/>
@@ -15526,52 +15470,44 @@
       <c r="I210" t="inlineStr"/>
       <c r="J210" t="inlineStr"/>
       <c r="K210" t="inlineStr"/>
-      <c r="L210" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M210" t="inlineStr"/>
-      <c r="N210" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L210" t="inlineStr"/>
+      <c r="M210" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N210" t="inlineStr"/>
       <c r="O210" t="inlineStr"/>
       <c r="P210" t="inlineStr"/>
-      <c r="Q210" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="Q210" t="inlineStr"/>
       <c r="R210" t="inlineStr"/>
       <c r="S210" t="inlineStr"/>
       <c r="T210" t="inlineStr"/>
       <c r="U210" t="inlineStr"/>
       <c r="V210" t="inlineStr">
         <is>
-          <t>EssnWrkP</t>
+          <t>NoIntP</t>
         </is>
       </c>
       <c r="W210" t="inlineStr">
         <is>
-          <t>Essential Workers %</t>
+          <t>Households without Internet Access %</t>
         </is>
       </c>
       <c r="X210" t="inlineStr"/>
       <c r="Y210" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Internet_Access.md</t>
         </is>
       </c>
       <c r="Z210" t="inlineStr">
         <is>
-          <t>ACS 2018, 2023</t>
+          <t>ACS 2019</t>
         </is>
       </c>
       <c r="AA210" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
+          <t>American Community Survey 2015-2019 5-Year Estimate</t>
         </is>
       </c>
       <c r="AB210" t="inlineStr"/>
@@ -15586,13 +15522,17 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Employment Trends</t>
+          <t>Poverty, Income, Gini Coefficient</t>
         </is>
       </c>
       <c r="C211" t="inlineStr"/>
       <c r="D211" t="inlineStr"/>
       <c r="E211" t="inlineStr"/>
-      <c r="F211" t="inlineStr"/>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G211" t="inlineStr"/>
       <c r="H211" t="inlineStr"/>
       <c r="I211" t="inlineStr"/>
@@ -15622,28 +15562,28 @@
       <c r="U211" t="inlineStr"/>
       <c r="V211" t="inlineStr">
         <is>
-          <t>HghRskP</t>
+          <t>MedInc</t>
         </is>
       </c>
       <c r="W211" t="inlineStr">
         <is>
-          <t>Employed % - High Risk of Injury</t>
+          <t>Median Income</t>
         </is>
       </c>
       <c r="X211" t="inlineStr"/>
       <c r="Y211" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Economic_Characteristics.md</t>
         </is>
       </c>
       <c r="Z211" t="inlineStr">
         <is>
-          <t>ACS 2018, 2023</t>
+          <t>ACS 2012, 2018; Social Explorer 2010</t>
         </is>
       </c>
       <c r="AA211" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
+          <t>American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates; Social Explorer Historic Census Data on 2010 Geographies</t>
         </is>
       </c>
       <c r="AB211" t="inlineStr"/>
@@ -15658,13 +15598,17 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Employment Trends</t>
+          <t>Poverty, Income, Gini Coefficient</t>
         </is>
       </c>
       <c r="C212" t="inlineStr"/>
       <c r="D212" t="inlineStr"/>
       <c r="E212" t="inlineStr"/>
-      <c r="F212" t="inlineStr"/>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G212" t="inlineStr"/>
       <c r="H212" t="inlineStr"/>
       <c r="I212" t="inlineStr"/>
@@ -15694,28 +15638,28 @@
       <c r="U212" t="inlineStr"/>
       <c r="V212" t="inlineStr">
         <is>
-          <t>HltCrP</t>
+          <t>PciE</t>
         </is>
       </c>
       <c r="W212" t="inlineStr">
         <is>
-          <t>Employed % - Health Care</t>
+          <t>Per Capita Income</t>
         </is>
       </c>
       <c r="X212" t="inlineStr"/>
       <c r="Y212" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Economic_Characteristics.md</t>
         </is>
       </c>
       <c r="Z212" t="inlineStr">
         <is>
-          <t>ACS 2018, 2023</t>
+          <t>ACS 2012, 2018; Social Explorer 2010</t>
         </is>
       </c>
       <c r="AA212" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
+          <t>American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates; Social Explorer Historic Census Data on 2010 Geographies</t>
         </is>
       </c>
       <c r="AB212" t="inlineStr"/>
@@ -15730,13 +15674,29 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Employment Trends</t>
-        </is>
-      </c>
-      <c r="C213" t="inlineStr"/>
-      <c r="D213" t="inlineStr"/>
-      <c r="E213" t="inlineStr"/>
-      <c r="F213" t="inlineStr"/>
+          <t>Poverty, Income, Gini Coefficient</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G213" t="inlineStr"/>
       <c r="H213" t="inlineStr"/>
       <c r="I213" t="inlineStr"/>
@@ -15763,31 +15723,35 @@
       <c r="R213" t="inlineStr"/>
       <c r="S213" t="inlineStr"/>
       <c r="T213" t="inlineStr"/>
-      <c r="U213" t="inlineStr"/>
+      <c r="U213" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="V213" t="inlineStr">
         <is>
-          <t>RetailP</t>
+          <t>PovP</t>
         </is>
       </c>
       <c r="W213" t="inlineStr">
         <is>
-          <t>Employed % - Retail</t>
+          <t>Poverty %</t>
         </is>
       </c>
       <c r="X213" t="inlineStr"/>
       <c r="Y213" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Economic_Characteristics.md</t>
         </is>
       </c>
       <c r="Z213" t="inlineStr">
         <is>
-          <t>ACS 2018, 2023</t>
+          <t>ACS 2012, 2018; Social Explorer 2010</t>
         </is>
       </c>
       <c r="AA213" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
+          <t>American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates; Social Explorer Historic Census Data on 2010 Geographies</t>
         </is>
       </c>
       <c r="AB213" t="inlineStr"/>
@@ -15802,13 +15766,29 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Employment Trends</t>
-        </is>
-      </c>
-      <c r="C214" t="inlineStr"/>
-      <c r="D214" t="inlineStr"/>
-      <c r="E214" t="inlineStr"/>
-      <c r="F214" t="inlineStr"/>
+          <t>Poverty, Income, Gini Coefficient</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G214" t="inlineStr"/>
       <c r="H214" t="inlineStr"/>
       <c r="I214" t="inlineStr"/>
@@ -15835,31 +15815,35 @@
       <c r="R214" t="inlineStr"/>
       <c r="S214" t="inlineStr"/>
       <c r="T214" t="inlineStr"/>
-      <c r="U214" t="inlineStr"/>
+      <c r="U214" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="V214" t="inlineStr">
         <is>
-          <t>TotWrkE</t>
+          <t>UnempP</t>
         </is>
       </c>
       <c r="W214" t="inlineStr">
         <is>
-          <t>Count of Working Population</t>
+          <t>Unemployment %</t>
         </is>
       </c>
       <c r="X214" t="inlineStr"/>
       <c r="Y214" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Employment_Trends.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Economic_Characteristics.md</t>
         </is>
       </c>
       <c r="Z214" t="inlineStr">
         <is>
-          <t>ACS 2018, 2023</t>
+          <t>ACS 2012, 2018; Social Explorer 2010</t>
         </is>
       </c>
       <c r="AA214" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 &amp; 2019-2023 5-Year Estimates</t>
+          <t>American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates; Social Explorer Historic Census Data on 2010 Geographies</t>
         </is>
       </c>
       <c r="AB214" t="inlineStr"/>
@@ -15869,12 +15853,12 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Economic</t>
+          <t>Outcome</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Great Recession Foreclosure Rate</t>
+          <t>Opioid Indicators</t>
         </is>
       </c>
       <c r="C215" t="inlineStr"/>
@@ -15882,19 +15866,51 @@
       <c r="E215" t="inlineStr"/>
       <c r="F215" t="inlineStr"/>
       <c r="G215" t="inlineStr"/>
-      <c r="H215" t="inlineStr"/>
-      <c r="I215" t="inlineStr"/>
-      <c r="J215" t="inlineStr"/>
-      <c r="K215" t="inlineStr"/>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J215" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L215" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="M215" t="inlineStr"/>
-      <c r="N215" t="inlineStr"/>
-      <c r="O215" t="inlineStr"/>
-      <c r="P215" t="inlineStr"/>
+      <c r="M215" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N215" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O215" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P215" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q215" t="inlineStr"/>
       <c r="R215" t="inlineStr"/>
       <c r="S215" t="inlineStr"/>
@@ -15902,28 +15918,28 @@
       <c r="U215" t="inlineStr"/>
       <c r="V215" t="inlineStr">
         <is>
-          <t>ForDqP</t>
+          <t>OdMortRt</t>
         </is>
       </c>
       <c r="W215" t="inlineStr">
         <is>
-          <t>Foreclosure &amp; Delinquency %</t>
+          <t>Overdose Mortality Rate</t>
         </is>
       </c>
       <c r="X215" t="inlineStr"/>
       <c r="Y215" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Foreclosure_Rate.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
         </is>
       </c>
       <c r="Z215" t="inlineStr">
         <is>
-          <t>HUD 2018; ACS 2012, 2018</t>
+          <t>HepVu 2014-2022</t>
         </is>
       </c>
       <c r="AA215" t="inlineStr">
         <is>
-          <t>U.S. Department of Housing and Urban Development Neighborhood Stabilization Program; American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates</t>
+          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
         </is>
       </c>
       <c r="AB215" t="inlineStr"/>
@@ -15933,12 +15949,12 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Economic</t>
+          <t>Outcome</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Great Recession Foreclosure Rate</t>
+          <t>Opioid Indicators</t>
         </is>
       </c>
       <c r="C216" t="inlineStr"/>
@@ -15950,13 +15966,13 @@
       <c r="I216" t="inlineStr"/>
       <c r="J216" t="inlineStr"/>
       <c r="K216" t="inlineStr"/>
-      <c r="L216" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L216" t="inlineStr"/>
       <c r="M216" t="inlineStr"/>
-      <c r="N216" t="inlineStr"/>
+      <c r="N216" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O216" t="inlineStr"/>
       <c r="P216" t="inlineStr"/>
       <c r="Q216" t="inlineStr"/>
@@ -15966,28 +15982,28 @@
       <c r="U216" t="inlineStr"/>
       <c r="V216" t="inlineStr">
         <is>
-          <t>ForDqTot</t>
+          <t>OdMortRtAv</t>
         </is>
       </c>
       <c r="W216" t="inlineStr">
         <is>
-          <t>Foreclosure &amp; Delinquency Count</t>
+          <t>Overdose Mortality Rate Average (2016-2020)</t>
         </is>
       </c>
       <c r="X216" t="inlineStr"/>
       <c r="Y216" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Foreclosure_Rate.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
         </is>
       </c>
       <c r="Z216" t="inlineStr">
         <is>
-          <t>HUD 2018; ACS 2012, 2018</t>
+          <t>HepVu 2014-2022</t>
         </is>
       </c>
       <c r="AA216" t="inlineStr">
         <is>
-          <t>U.S. Department of Housing and Urban Development Neighborhood Stabilization Program; American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates</t>
+          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
         </is>
       </c>
       <c r="AB216" t="inlineStr"/>
@@ -15997,32 +16013,24 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Economic</t>
+          <t>Outcome</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Great Recession Foreclosure Rate</t>
+          <t>Opioid Indicators</t>
         </is>
       </c>
       <c r="C217" t="inlineStr"/>
       <c r="D217" t="inlineStr"/>
       <c r="E217" t="inlineStr"/>
-      <c r="F217" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F217" t="inlineStr"/>
       <c r="G217" t="inlineStr"/>
       <c r="H217" t="inlineStr"/>
       <c r="I217" t="inlineStr"/>
       <c r="J217" t="inlineStr"/>
       <c r="K217" t="inlineStr"/>
-      <c r="L217" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L217" t="inlineStr"/>
       <c r="M217" t="inlineStr"/>
       <c r="N217" t="inlineStr">
         <is>
@@ -16030,40 +16038,40 @@
         </is>
       </c>
       <c r="O217" t="inlineStr"/>
-      <c r="P217" t="inlineStr"/>
-      <c r="Q217" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P217" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q217" t="inlineStr"/>
       <c r="R217" t="inlineStr"/>
       <c r="S217" t="inlineStr"/>
       <c r="T217" t="inlineStr"/>
       <c r="U217" t="inlineStr"/>
       <c r="V217" t="inlineStr">
         <is>
-          <t>GiniCoeff</t>
+          <t>OpRxRt</t>
         </is>
       </c>
       <c r="W217" t="inlineStr">
         <is>
-          <t>Income Inequality (Gini Coefficient)</t>
+          <t>Opioid Prescription Rate</t>
         </is>
       </c>
       <c r="X217" t="inlineStr"/>
       <c r="Y217" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Foreclosure_Rate.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
         </is>
       </c>
       <c r="Z217" t="inlineStr">
         <is>
-          <t>HUD 2018; ACS 2012, 2018</t>
+          <t>HepVu 2014-2022</t>
         </is>
       </c>
       <c r="AA217" t="inlineStr">
         <is>
-          <t>U.S. Department of Housing and Urban Development Neighborhood Stabilization Program; American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates</t>
+          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
         </is>
       </c>
       <c r="AB217" t="inlineStr"/>
@@ -16073,12 +16081,12 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Economic</t>
+          <t>Composite</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Internet Access</t>
+          <t>Social Vulnerability Indices</t>
         </is>
       </c>
       <c r="C218" t="inlineStr"/>
@@ -16090,15 +16098,23 @@
       <c r="I218" t="inlineStr"/>
       <c r="J218" t="inlineStr"/>
       <c r="K218" t="inlineStr"/>
-      <c r="L218" t="inlineStr"/>
-      <c r="M218" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N218" t="inlineStr"/>
+      <c r="L218" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M218" t="inlineStr"/>
+      <c r="N218" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O218" t="inlineStr"/>
-      <c r="P218" t="inlineStr"/>
+      <c r="P218" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q218" t="inlineStr"/>
       <c r="R218" t="inlineStr"/>
       <c r="S218" t="inlineStr"/>
@@ -16106,28 +16122,28 @@
       <c r="U218" t="inlineStr"/>
       <c r="V218" t="inlineStr">
         <is>
-          <t>NoIntP</t>
+          <t>SviSmryRnk</t>
         </is>
       </c>
       <c r="W218" t="inlineStr">
         <is>
-          <t>Households without Internet Access %</t>
+          <t>Social Vulnerability Index (SVI) Summary Ranking</t>
         </is>
       </c>
       <c r="X218" t="inlineStr"/>
       <c r="Y218" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Internet_Access.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Social_Vulnerability_Indices.md</t>
         </is>
       </c>
       <c r="Z218" t="inlineStr">
         <is>
-          <t>ACS 2019</t>
+          <t>CDC 2018, 2020, 2022</t>
         </is>
       </c>
       <c r="AA218" t="inlineStr">
         <is>
-          <t>American Community Survey 2015-2019 5-Year Estimate</t>
+          <t>Centers for Disease Control, 2018, 2020, 2022</t>
         </is>
       </c>
       <c r="AB218" t="inlineStr"/>
@@ -16137,22 +16153,18 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Economic</t>
+          <t>Composite</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Poverty, Income, Gini Coefficient</t>
+          <t>Social Vulnerability Indices</t>
         </is>
       </c>
       <c r="C219" t="inlineStr"/>
       <c r="D219" t="inlineStr"/>
       <c r="E219" t="inlineStr"/>
-      <c r="F219" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F219" t="inlineStr"/>
       <c r="G219" t="inlineStr"/>
       <c r="H219" t="inlineStr"/>
       <c r="I219" t="inlineStr"/>
@@ -16170,40 +16182,44 @@
         </is>
       </c>
       <c r="O219" t="inlineStr"/>
-      <c r="P219" t="inlineStr"/>
-      <c r="Q219" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P219" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q219" t="inlineStr"/>
       <c r="R219" t="inlineStr"/>
       <c r="S219" t="inlineStr"/>
-      <c r="T219" t="inlineStr"/>
+      <c r="T219" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U219" t="inlineStr"/>
       <c r="V219" t="inlineStr">
         <is>
-          <t>MedInc</t>
+          <t>SviTh1</t>
         </is>
       </c>
       <c r="W219" t="inlineStr">
         <is>
-          <t>Median Income</t>
+          <t>Social Vulnerability Index (SVI) 1</t>
         </is>
       </c>
       <c r="X219" t="inlineStr"/>
       <c r="Y219" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Economic_Characteristics.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Social_Vulnerability_Indices.md</t>
         </is>
       </c>
       <c r="Z219" t="inlineStr">
         <is>
-          <t>ACS 2012, 2018; Social Explorer 2010</t>
+          <t>CDC 2018, 2020, 2022</t>
         </is>
       </c>
       <c r="AA219" t="inlineStr">
         <is>
-          <t>American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates; Social Explorer Historic Census Data on 2010 Geographies</t>
+          <t>Centers for Disease Control, 2018, 2020, 2022</t>
         </is>
       </c>
       <c r="AB219" t="inlineStr"/>
@@ -16213,22 +16229,18 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Economic</t>
+          <t>Composite</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Poverty, Income, Gini Coefficient</t>
+          <t>Social Vulnerability Indices</t>
         </is>
       </c>
       <c r="C220" t="inlineStr"/>
       <c r="D220" t="inlineStr"/>
       <c r="E220" t="inlineStr"/>
-      <c r="F220" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F220" t="inlineStr"/>
       <c r="G220" t="inlineStr"/>
       <c r="H220" t="inlineStr"/>
       <c r="I220" t="inlineStr"/>
@@ -16246,40 +16258,40 @@
         </is>
       </c>
       <c r="O220" t="inlineStr"/>
-      <c r="P220" t="inlineStr"/>
-      <c r="Q220" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P220" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q220" t="inlineStr"/>
       <c r="R220" t="inlineStr"/>
       <c r="S220" t="inlineStr"/>
       <c r="T220" t="inlineStr"/>
       <c r="U220" t="inlineStr"/>
       <c r="V220" t="inlineStr">
         <is>
-          <t>PciE</t>
+          <t>SviTh2</t>
         </is>
       </c>
       <c r="W220" t="inlineStr">
         <is>
-          <t>Per Capita Income</t>
+          <t>Social Vulnerability Index (SVI) 2</t>
         </is>
       </c>
       <c r="X220" t="inlineStr"/>
       <c r="Y220" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Economic_Characteristics.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Social_Vulnerability_Indices.md</t>
         </is>
       </c>
       <c r="Z220" t="inlineStr">
         <is>
-          <t>ACS 2012, 2018; Social Explorer 2010</t>
+          <t>CDC 2018, 2020, 2022</t>
         </is>
       </c>
       <c r="AA220" t="inlineStr">
         <is>
-          <t>American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates; Social Explorer Historic Census Data on 2010 Geographies</t>
+          <t>Centers for Disease Control, 2018, 2020, 2022</t>
         </is>
       </c>
       <c r="AB220" t="inlineStr"/>
@@ -16289,34 +16301,18 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Economic</t>
+          <t>Composite</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Poverty, Income, Gini Coefficient</t>
-        </is>
-      </c>
-      <c r="C221" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D221" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E221" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="F221" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+          <t>Social Vulnerability Indices</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr"/>
+      <c r="D221" t="inlineStr"/>
+      <c r="E221" t="inlineStr"/>
+      <c r="F221" t="inlineStr"/>
       <c r="G221" t="inlineStr"/>
       <c r="H221" t="inlineStr"/>
       <c r="I221" t="inlineStr"/>
@@ -16334,44 +16330,40 @@
         </is>
       </c>
       <c r="O221" t="inlineStr"/>
-      <c r="P221" t="inlineStr"/>
-      <c r="Q221" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P221" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q221" t="inlineStr"/>
       <c r="R221" t="inlineStr"/>
       <c r="S221" t="inlineStr"/>
       <c r="T221" t="inlineStr"/>
-      <c r="U221" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="U221" t="inlineStr"/>
       <c r="V221" t="inlineStr">
         <is>
-          <t>PovP</t>
+          <t>SviTh3</t>
         </is>
       </c>
       <c r="W221" t="inlineStr">
         <is>
-          <t>Poverty %</t>
+          <t>Social Vulnerability Index (SVI) 3</t>
         </is>
       </c>
       <c r="X221" t="inlineStr"/>
       <c r="Y221" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Economic_Characteristics.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Social_Vulnerability_Indices.md</t>
         </is>
       </c>
       <c r="Z221" t="inlineStr">
         <is>
-          <t>ACS 2012, 2018; Social Explorer 2010</t>
+          <t>CDC 2018, 2020, 2022</t>
         </is>
       </c>
       <c r="AA221" t="inlineStr">
         <is>
-          <t>American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates; Social Explorer Historic Census Data on 2010 Geographies</t>
+          <t>Centers for Disease Control, 2018, 2020, 2022</t>
         </is>
       </c>
       <c r="AB221" t="inlineStr"/>
@@ -16381,34 +16373,18 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Economic</t>
+          <t>Composite</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Poverty, Income, Gini Coefficient</t>
-        </is>
-      </c>
-      <c r="C222" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D222" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E222" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="F222" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+          <t>Social Vulnerability Indices</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr"/>
+      <c r="D222" t="inlineStr"/>
+      <c r="E222" t="inlineStr"/>
+      <c r="F222" t="inlineStr"/>
       <c r="G222" t="inlineStr"/>
       <c r="H222" t="inlineStr"/>
       <c r="I222" t="inlineStr"/>
@@ -16426,645 +16402,49 @@
         </is>
       </c>
       <c r="O222" t="inlineStr"/>
-      <c r="P222" t="inlineStr"/>
-      <c r="Q222" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P222" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q222" t="inlineStr"/>
       <c r="R222" t="inlineStr"/>
       <c r="S222" t="inlineStr"/>
-      <c r="T222" t="inlineStr"/>
-      <c r="U222" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="T222" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="U222" t="inlineStr"/>
       <c r="V222" t="inlineStr">
         <is>
-          <t>UnempP</t>
+          <t>SviTh4</t>
         </is>
       </c>
       <c r="W222" t="inlineStr">
         <is>
-          <t>Unemployment %</t>
+          <t>Social Vulnerability Index (SVI) 4</t>
         </is>
       </c>
       <c r="X222" t="inlineStr"/>
       <c r="Y222" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Economic_Characteristics.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Social_Vulnerability_Indices.md</t>
         </is>
       </c>
       <c r="Z222" t="inlineStr">
         <is>
-          <t>ACS 2012, 2018; Social Explorer 2010</t>
+          <t>CDC 2018, 2020, 2022</t>
         </is>
       </c>
       <c r="AA222" t="inlineStr">
         <is>
-          <t>American Community Survey 2008-2012 &amp; 2014-2018 5-Year Estimates; Social Explorer Historic Census Data on 2010 Geographies</t>
+          <t>Centers for Disease Control, 2018, 2020, 2022</t>
         </is>
       </c>
       <c r="AB222" t="inlineStr"/>
       <c r="AC222" t="inlineStr"/>
       <c r="AD222" t="inlineStr"/>
-    </row>
-    <row r="223">
-      <c r="A223" t="inlineStr">
-        <is>
-          <t>Outcome</t>
-        </is>
-      </c>
-      <c r="B223" t="inlineStr">
-        <is>
-          <t>Opioid Indicators</t>
-        </is>
-      </c>
-      <c r="C223" t="inlineStr"/>
-      <c r="D223" t="inlineStr"/>
-      <c r="E223" t="inlineStr"/>
-      <c r="F223" t="inlineStr"/>
-      <c r="G223" t="inlineStr"/>
-      <c r="H223" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I223" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J223" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K223" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L223" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M223" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N223" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O223" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P223" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q223" t="inlineStr"/>
-      <c r="R223" t="inlineStr"/>
-      <c r="S223" t="inlineStr"/>
-      <c r="T223" t="inlineStr"/>
-      <c r="U223" t="inlineStr"/>
-      <c r="V223" t="inlineStr">
-        <is>
-          <t>OdMortRt</t>
-        </is>
-      </c>
-      <c r="W223" t="inlineStr">
-        <is>
-          <t>Overdose Mortality Rate</t>
-        </is>
-      </c>
-      <c r="X223" t="inlineStr"/>
-      <c r="Y223" t="inlineStr">
-        <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
-        </is>
-      </c>
-      <c r="Z223" t="inlineStr">
-        <is>
-          <t>HepVu 2014-2022</t>
-        </is>
-      </c>
-      <c r="AA223" t="inlineStr">
-        <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
-        </is>
-      </c>
-      <c r="AB223" t="inlineStr"/>
-      <c r="AC223" t="inlineStr"/>
-      <c r="AD223" t="inlineStr"/>
-    </row>
-    <row r="224">
-      <c r="A224" t="inlineStr">
-        <is>
-          <t>Outcome</t>
-        </is>
-      </c>
-      <c r="B224" t="inlineStr">
-        <is>
-          <t>Opioid Indicators</t>
-        </is>
-      </c>
-      <c r="C224" t="inlineStr"/>
-      <c r="D224" t="inlineStr"/>
-      <c r="E224" t="inlineStr"/>
-      <c r="F224" t="inlineStr"/>
-      <c r="G224" t="inlineStr"/>
-      <c r="H224" t="inlineStr"/>
-      <c r="I224" t="inlineStr"/>
-      <c r="J224" t="inlineStr"/>
-      <c r="K224" t="inlineStr"/>
-      <c r="L224" t="inlineStr"/>
-      <c r="M224" t="inlineStr"/>
-      <c r="N224" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O224" t="inlineStr"/>
-      <c r="P224" t="inlineStr"/>
-      <c r="Q224" t="inlineStr"/>
-      <c r="R224" t="inlineStr"/>
-      <c r="S224" t="inlineStr"/>
-      <c r="T224" t="inlineStr"/>
-      <c r="U224" t="inlineStr"/>
-      <c r="V224" t="inlineStr">
-        <is>
-          <t>OdMortRtAv</t>
-        </is>
-      </c>
-      <c r="W224" t="inlineStr">
-        <is>
-          <t>Overdose Mortality Rate Average (2016-2020)</t>
-        </is>
-      </c>
-      <c r="X224" t="inlineStr"/>
-      <c r="Y224" t="inlineStr">
-        <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
-        </is>
-      </c>
-      <c r="Z224" t="inlineStr">
-        <is>
-          <t>HepVu 2014-2022</t>
-        </is>
-      </c>
-      <c r="AA224" t="inlineStr">
-        <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
-        </is>
-      </c>
-      <c r="AB224" t="inlineStr"/>
-      <c r="AC224" t="inlineStr"/>
-      <c r="AD224" t="inlineStr"/>
-    </row>
-    <row r="225">
-      <c r="A225" t="inlineStr">
-        <is>
-          <t>Outcome</t>
-        </is>
-      </c>
-      <c r="B225" t="inlineStr">
-        <is>
-          <t>Opioid Indicators</t>
-        </is>
-      </c>
-      <c r="C225" t="inlineStr"/>
-      <c r="D225" t="inlineStr"/>
-      <c r="E225" t="inlineStr"/>
-      <c r="F225" t="inlineStr"/>
-      <c r="G225" t="inlineStr"/>
-      <c r="H225" t="inlineStr"/>
-      <c r="I225" t="inlineStr"/>
-      <c r="J225" t="inlineStr"/>
-      <c r="K225" t="inlineStr"/>
-      <c r="L225" t="inlineStr"/>
-      <c r="M225" t="inlineStr"/>
-      <c r="N225" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O225" t="inlineStr"/>
-      <c r="P225" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q225" t="inlineStr"/>
-      <c r="R225" t="inlineStr"/>
-      <c r="S225" t="inlineStr"/>
-      <c r="T225" t="inlineStr"/>
-      <c r="U225" t="inlineStr"/>
-      <c r="V225" t="inlineStr">
-        <is>
-          <t>OpRxRt</t>
-        </is>
-      </c>
-      <c r="W225" t="inlineStr">
-        <is>
-          <t>Opioid Prescription Rate</t>
-        </is>
-      </c>
-      <c r="X225" t="inlineStr"/>
-      <c r="Y225" t="inlineStr">
-        <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
-        </is>
-      </c>
-      <c r="Z225" t="inlineStr">
-        <is>
-          <t>HepVu 2014-2022</t>
-        </is>
-      </c>
-      <c r="AA225" t="inlineStr">
-        <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
-        </is>
-      </c>
-      <c r="AB225" t="inlineStr"/>
-      <c r="AC225" t="inlineStr"/>
-      <c r="AD225" t="inlineStr"/>
-    </row>
-    <row r="226">
-      <c r="A226" t="inlineStr">
-        <is>
-          <t>Composite</t>
-        </is>
-      </c>
-      <c r="B226" t="inlineStr">
-        <is>
-          <t>Social Vulnerability Indices</t>
-        </is>
-      </c>
-      <c r="C226" t="inlineStr"/>
-      <c r="D226" t="inlineStr"/>
-      <c r="E226" t="inlineStr"/>
-      <c r="F226" t="inlineStr"/>
-      <c r="G226" t="inlineStr"/>
-      <c r="H226" t="inlineStr"/>
-      <c r="I226" t="inlineStr"/>
-      <c r="J226" t="inlineStr"/>
-      <c r="K226" t="inlineStr"/>
-      <c r="L226" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M226" t="inlineStr"/>
-      <c r="N226" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O226" t="inlineStr"/>
-      <c r="P226" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q226" t="inlineStr"/>
-      <c r="R226" t="inlineStr"/>
-      <c r="S226" t="inlineStr"/>
-      <c r="T226" t="inlineStr"/>
-      <c r="U226" t="inlineStr"/>
-      <c r="V226" t="inlineStr">
-        <is>
-          <t>SviSmryRnk</t>
-        </is>
-      </c>
-      <c r="W226" t="inlineStr">
-        <is>
-          <t>Social Vulnerability Index (SVI) Summary Ranking</t>
-        </is>
-      </c>
-      <c r="X226" t="inlineStr"/>
-      <c r="Y226" t="inlineStr">
-        <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Social_Vulnerability_Indices.md</t>
-        </is>
-      </c>
-      <c r="Z226" t="inlineStr">
-        <is>
-          <t>CDC 2018, 2020, 2022</t>
-        </is>
-      </c>
-      <c r="AA226" t="inlineStr">
-        <is>
-          <t>Centers for Disease Control, 2018, 2020, 2022</t>
-        </is>
-      </c>
-      <c r="AB226" t="inlineStr"/>
-      <c r="AC226" t="inlineStr"/>
-      <c r="AD226" t="inlineStr"/>
-    </row>
-    <row r="227">
-      <c r="A227" t="inlineStr">
-        <is>
-          <t>Composite</t>
-        </is>
-      </c>
-      <c r="B227" t="inlineStr">
-        <is>
-          <t>Social Vulnerability Indices</t>
-        </is>
-      </c>
-      <c r="C227" t="inlineStr"/>
-      <c r="D227" t="inlineStr"/>
-      <c r="E227" t="inlineStr"/>
-      <c r="F227" t="inlineStr"/>
-      <c r="G227" t="inlineStr"/>
-      <c r="H227" t="inlineStr"/>
-      <c r="I227" t="inlineStr"/>
-      <c r="J227" t="inlineStr"/>
-      <c r="K227" t="inlineStr"/>
-      <c r="L227" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M227" t="inlineStr"/>
-      <c r="N227" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O227" t="inlineStr"/>
-      <c r="P227" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q227" t="inlineStr"/>
-      <c r="R227" t="inlineStr"/>
-      <c r="S227" t="inlineStr"/>
-      <c r="T227" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="U227" t="inlineStr"/>
-      <c r="V227" t="inlineStr">
-        <is>
-          <t>SviTh1</t>
-        </is>
-      </c>
-      <c r="W227" t="inlineStr">
-        <is>
-          <t>Social Vulnerability Index (SVI) 1</t>
-        </is>
-      </c>
-      <c r="X227" t="inlineStr"/>
-      <c r="Y227" t="inlineStr">
-        <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Social_Vulnerability_Indices.md</t>
-        </is>
-      </c>
-      <c r="Z227" t="inlineStr">
-        <is>
-          <t>CDC 2018, 2020, 2022</t>
-        </is>
-      </c>
-      <c r="AA227" t="inlineStr">
-        <is>
-          <t>Centers for Disease Control, 2018, 2020, 2022</t>
-        </is>
-      </c>
-      <c r="AB227" t="inlineStr"/>
-      <c r="AC227" t="inlineStr"/>
-      <c r="AD227" t="inlineStr"/>
-    </row>
-    <row r="228">
-      <c r="A228" t="inlineStr">
-        <is>
-          <t>Composite</t>
-        </is>
-      </c>
-      <c r="B228" t="inlineStr">
-        <is>
-          <t>Social Vulnerability Indices</t>
-        </is>
-      </c>
-      <c r="C228" t="inlineStr"/>
-      <c r="D228" t="inlineStr"/>
-      <c r="E228" t="inlineStr"/>
-      <c r="F228" t="inlineStr"/>
-      <c r="G228" t="inlineStr"/>
-      <c r="H228" t="inlineStr"/>
-      <c r="I228" t="inlineStr"/>
-      <c r="J228" t="inlineStr"/>
-      <c r="K228" t="inlineStr"/>
-      <c r="L228" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M228" t="inlineStr"/>
-      <c r="N228" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O228" t="inlineStr"/>
-      <c r="P228" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q228" t="inlineStr"/>
-      <c r="R228" t="inlineStr"/>
-      <c r="S228" t="inlineStr"/>
-      <c r="T228" t="inlineStr"/>
-      <c r="U228" t="inlineStr"/>
-      <c r="V228" t="inlineStr">
-        <is>
-          <t>SviTh2</t>
-        </is>
-      </c>
-      <c r="W228" t="inlineStr">
-        <is>
-          <t>Social Vulnerability Index (SVI) 2</t>
-        </is>
-      </c>
-      <c r="X228" t="inlineStr"/>
-      <c r="Y228" t="inlineStr">
-        <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Social_Vulnerability_Indices.md</t>
-        </is>
-      </c>
-      <c r="Z228" t="inlineStr">
-        <is>
-          <t>CDC 2018, 2020, 2022</t>
-        </is>
-      </c>
-      <c r="AA228" t="inlineStr">
-        <is>
-          <t>Centers for Disease Control, 2018, 2020, 2022</t>
-        </is>
-      </c>
-      <c r="AB228" t="inlineStr"/>
-      <c r="AC228" t="inlineStr"/>
-      <c r="AD228" t="inlineStr"/>
-    </row>
-    <row r="229">
-      <c r="A229" t="inlineStr">
-        <is>
-          <t>Composite</t>
-        </is>
-      </c>
-      <c r="B229" t="inlineStr">
-        <is>
-          <t>Social Vulnerability Indices</t>
-        </is>
-      </c>
-      <c r="C229" t="inlineStr"/>
-      <c r="D229" t="inlineStr"/>
-      <c r="E229" t="inlineStr"/>
-      <c r="F229" t="inlineStr"/>
-      <c r="G229" t="inlineStr"/>
-      <c r="H229" t="inlineStr"/>
-      <c r="I229" t="inlineStr"/>
-      <c r="J229" t="inlineStr"/>
-      <c r="K229" t="inlineStr"/>
-      <c r="L229" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M229" t="inlineStr"/>
-      <c r="N229" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O229" t="inlineStr"/>
-      <c r="P229" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q229" t="inlineStr"/>
-      <c r="R229" t="inlineStr"/>
-      <c r="S229" t="inlineStr"/>
-      <c r="T229" t="inlineStr"/>
-      <c r="U229" t="inlineStr"/>
-      <c r="V229" t="inlineStr">
-        <is>
-          <t>SviTh3</t>
-        </is>
-      </c>
-      <c r="W229" t="inlineStr">
-        <is>
-          <t>Social Vulnerability Index (SVI) 3</t>
-        </is>
-      </c>
-      <c r="X229" t="inlineStr"/>
-      <c r="Y229" t="inlineStr">
-        <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Social_Vulnerability_Indices.md</t>
-        </is>
-      </c>
-      <c r="Z229" t="inlineStr">
-        <is>
-          <t>CDC 2018, 2020, 2022</t>
-        </is>
-      </c>
-      <c r="AA229" t="inlineStr">
-        <is>
-          <t>Centers for Disease Control, 2018, 2020, 2022</t>
-        </is>
-      </c>
-      <c r="AB229" t="inlineStr"/>
-      <c r="AC229" t="inlineStr"/>
-      <c r="AD229" t="inlineStr"/>
-    </row>
-    <row r="230">
-      <c r="A230" t="inlineStr">
-        <is>
-          <t>Composite</t>
-        </is>
-      </c>
-      <c r="B230" t="inlineStr">
-        <is>
-          <t>Social Vulnerability Indices</t>
-        </is>
-      </c>
-      <c r="C230" t="inlineStr"/>
-      <c r="D230" t="inlineStr"/>
-      <c r="E230" t="inlineStr"/>
-      <c r="F230" t="inlineStr"/>
-      <c r="G230" t="inlineStr"/>
-      <c r="H230" t="inlineStr"/>
-      <c r="I230" t="inlineStr"/>
-      <c r="J230" t="inlineStr"/>
-      <c r="K230" t="inlineStr"/>
-      <c r="L230" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M230" t="inlineStr"/>
-      <c r="N230" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O230" t="inlineStr"/>
-      <c r="P230" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q230" t="inlineStr"/>
-      <c r="R230" t="inlineStr"/>
-      <c r="S230" t="inlineStr"/>
-      <c r="T230" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="U230" t="inlineStr"/>
-      <c r="V230" t="inlineStr">
-        <is>
-          <t>SviTh4</t>
-        </is>
-      </c>
-      <c r="W230" t="inlineStr">
-        <is>
-          <t>Social Vulnerability Index (SVI) 4</t>
-        </is>
-      </c>
-      <c r="X230" t="inlineStr"/>
-      <c r="Y230" t="inlineStr">
-        <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Social_Vulnerability_Indices.md</t>
-        </is>
-      </c>
-      <c r="Z230" t="inlineStr">
-        <is>
-          <t>CDC 2018, 2020, 2022</t>
-        </is>
-      </c>
-      <c r="AA230" t="inlineStr">
-        <is>
-          <t>Centers for Disease Control, 2018, 2020, 2022</t>
-        </is>
-      </c>
-      <c r="AB230" t="inlineStr"/>
-      <c r="AC230" t="inlineStr"/>
-      <c r="AD230" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>